<commit_message>
corrected 2020 to 20 in date
</commit_message>
<xml_diff>
--- a/fastqFiles/fastqFiles_10.19.20.xlsx
+++ b/fastqFiles/fastqFiles_10.19.20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/fastqFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8002BB8-0C39-9047-8E54-CEC1094CD243}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A781DA1-2670-D84A-AE73-797F3AD27066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="500" windowWidth="24860" windowHeight="19760" xr2:uid="{BB0EF9DB-E5D8-EA44-A68D-849CB4CFC21E}"/>
+    <workbookView xWindow="8740" yWindow="460" windowWidth="24860" windowHeight="19120" xr2:uid="{BB0EF9DB-E5D8-EA44-A68D-849CB4CFC21E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -71,9 +63,6 @@
     <t>fastqFileName</t>
   </si>
   <si>
-    <t>10.05.2020</t>
-  </si>
-  <si>
     <t>J.PLAGGENBERG</t>
   </si>
   <si>
@@ -243,6 +232,9 @@
   </si>
   <si>
     <t>Brent_Exp29-24_GTAC_24_SIC_Index2_08_GGAGTCC_AAGCACGT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>10.05.20</t>
   </si>
 </sst>
 </file>
@@ -597,7 +589,7 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,10 +637,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -657,13 +649,13 @@
         <v>4632</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2">
         <v>0.55900000000000005</v>
@@ -675,15 +667,15 @@
         <v>216359</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -692,13 +684,13 @@
         <v>4632</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>2.25</v>
@@ -710,15 +702,15 @@
         <v>345550</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -727,13 +719,13 @@
         <v>4632</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>0.35499999999999998</v>
@@ -745,15 +737,15 @@
         <v>646576</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -762,13 +754,13 @@
         <v>4632</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <v>1.58</v>
@@ -780,15 +772,15 @@
         <v>6955921</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -797,13 +789,13 @@
         <v>4632</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>51</v>
@@ -815,15 +807,15 @@
         <v>14054487</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -832,13 +824,13 @@
         <v>4632</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7">
         <v>0.22700000000000001</v>
@@ -850,15 +842,15 @@
         <v>321935</v>
       </c>
       <c r="L7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -867,13 +859,13 @@
         <v>4632</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>22</v>
@@ -885,15 +877,15 @@
         <v>9386053</v>
       </c>
       <c r="L8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -902,13 +894,13 @@
         <v>4632</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9">
         <v>11.6</v>
@@ -920,15 +912,15 @@
         <v>7252282</v>
       </c>
       <c r="L9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -937,13 +929,13 @@
         <v>4632</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10">
         <v>0.248</v>
@@ -955,15 +947,15 @@
         <v>343550</v>
       </c>
       <c r="L10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -972,13 +964,13 @@
         <v>4632</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11">
         <v>0.30199999999999999</v>
@@ -990,15 +982,15 @@
         <v>490360</v>
       </c>
       <c r="L11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -1007,13 +999,13 @@
         <v>4632</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I12">
         <v>29.4</v>
@@ -1025,15 +1017,15 @@
         <v>9341321</v>
       </c>
       <c r="L12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -1042,13 +1034,13 @@
         <v>4632</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13">
         <v>21.2</v>
@@ -1060,15 +1052,15 @@
         <v>1571825</v>
       </c>
       <c r="L13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -1077,13 +1069,13 @@
         <v>4632</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14">
         <v>36.700000000000003</v>
@@ -1095,15 +1087,15 @@
         <v>9184269</v>
       </c>
       <c r="L14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1112,13 +1104,13 @@
         <v>4632</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I15">
         <v>2.57</v>
@@ -1130,15 +1122,15 @@
         <v>9089593</v>
       </c>
       <c r="L15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -1147,13 +1139,13 @@
         <v>4632</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I16">
         <v>38.9</v>
@@ -1165,15 +1157,15 @@
         <v>9252451</v>
       </c>
       <c r="L16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -1182,13 +1174,13 @@
         <v>4632</v>
       </c>
       <c r="F17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I17">
         <v>15.9</v>
@@ -1200,15 +1192,15 @@
         <v>10899777</v>
       </c>
       <c r="L17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -1217,13 +1209,13 @@
         <v>4632</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I18">
         <v>1.85</v>
@@ -1235,15 +1227,15 @@
         <v>154349</v>
       </c>
       <c r="L18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -1252,13 +1244,13 @@
         <v>4632</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I19">
         <v>0.36599999999999999</v>
@@ -1270,15 +1262,15 @@
         <v>339088</v>
       </c>
       <c r="L19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -1287,13 +1279,13 @@
         <v>4632</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I20">
         <v>2.42</v>
@@ -1305,15 +1297,15 @@
         <v>9979665</v>
       </c>
       <c r="L20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1322,13 +1314,13 @@
         <v>4632</v>
       </c>
       <c r="F21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I21">
         <v>1.07</v>
@@ -1340,15 +1332,15 @@
         <v>351263</v>
       </c>
       <c r="L21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -1357,13 +1349,13 @@
         <v>4632</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I22">
         <v>31.2</v>
@@ -1375,15 +1367,15 @@
         <v>10592397</v>
       </c>
       <c r="L22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -1392,13 +1384,13 @@
         <v>4632</v>
       </c>
       <c r="F23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I23">
         <v>32.5</v>
@@ -1410,15 +1402,15 @@
         <v>9832585</v>
       </c>
       <c r="L23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -1427,13 +1419,13 @@
         <v>4632</v>
       </c>
       <c r="F24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I24">
         <v>17.5</v>
@@ -1445,15 +1437,15 @@
         <v>11093440</v>
       </c>
       <c r="L24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -1462,13 +1454,13 @@
         <v>4632</v>
       </c>
       <c r="F25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I25">
         <v>14.9</v>
@@ -1480,15 +1472,15 @@
         <v>12084614</v>
       </c>
       <c r="L25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -1497,13 +1489,13 @@
         <v>4632</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I26">
         <v>16.100000000000001</v>
@@ -1515,15 +1507,15 @@
         <v>9861043</v>
       </c>
       <c r="L26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -1532,13 +1524,13 @@
         <v>4632</v>
       </c>
       <c r="F27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I27">
         <v>0.31</v>
@@ -1550,15 +1542,15 @@
         <v>1026585</v>
       </c>
       <c r="L27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -1567,13 +1559,13 @@
         <v>4632</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I28">
         <v>3.32</v>
@@ -1585,15 +1577,15 @@
         <v>10030674</v>
       </c>
       <c r="L28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -1602,13 +1594,13 @@
         <v>4632</v>
       </c>
       <c r="F29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I29">
         <v>0.30099999999999999</v>
@@ -1620,15 +1612,15 @@
         <v>604426</v>
       </c>
       <c r="L29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1637,13 +1629,13 @@
         <v>4632</v>
       </c>
       <c r="F30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I30">
         <v>4.1500000000000004</v>
@@ -1655,15 +1647,15 @@
         <v>7432800</v>
       </c>
       <c r="L30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1672,13 +1664,13 @@
         <v>4632</v>
       </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I31">
         <v>15.8</v>
@@ -1690,15 +1682,15 @@
         <v>9835980</v>
       </c>
       <c r="L31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1707,13 +1699,13 @@
         <v>4632</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I32">
         <v>0.32900000000000001</v>
@@ -1725,15 +1717,15 @@
         <v>1853051</v>
       </c>
       <c r="L32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1742,13 +1734,13 @@
         <v>4632</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I33">
         <v>9.83</v>
@@ -1760,15 +1752,15 @@
         <v>2916440</v>
       </c>
       <c r="L33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>5</v>
@@ -1777,13 +1769,13 @@
         <v>4632</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I34">
         <v>3.19</v>
@@ -1795,15 +1787,15 @@
         <v>12415090</v>
       </c>
       <c r="L34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C35">
         <v>6</v>
@@ -1812,13 +1804,13 @@
         <v>4632</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I35">
         <v>5.54</v>
@@ -1830,15 +1822,15 @@
         <v>6327046</v>
       </c>
       <c r="L35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C36">
         <v>7</v>
@@ -1847,13 +1839,13 @@
         <v>4632</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I36">
         <v>0.60699999999999998</v>
@@ -1865,15 +1857,15 @@
         <v>1878084</v>
       </c>
       <c r="L36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C37">
         <v>8</v>
@@ -1882,13 +1874,13 @@
         <v>4632</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I37">
         <v>3.46</v>
@@ -1900,15 +1892,15 @@
         <v>11284684</v>
       </c>
       <c r="L37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C38">
         <v>9</v>
@@ -1917,13 +1909,13 @@
         <v>4632</v>
       </c>
       <c r="F38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I38">
         <v>0.874</v>
@@ -1935,15 +1927,15 @@
         <v>2009550</v>
       </c>
       <c r="L38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -1952,13 +1944,13 @@
         <v>4632</v>
       </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I39">
         <v>1.44</v>
@@ -1970,15 +1962,15 @@
         <v>7696088</v>
       </c>
       <c r="L39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C40">
         <v>11</v>
@@ -1987,13 +1979,13 @@
         <v>4632</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I40">
         <v>19.100000000000001</v>
@@ -2005,15 +1997,15 @@
         <v>10650271</v>
       </c>
       <c r="L40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -2022,13 +2014,13 @@
         <v>4632</v>
       </c>
       <c r="F41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I41">
         <v>18.399999999999999</v>
@@ -2040,15 +2032,15 @@
         <v>10456927</v>
       </c>
       <c r="L41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C42">
         <v>13</v>
@@ -2057,13 +2049,13 @@
         <v>4632</v>
       </c>
       <c r="F42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I42">
         <v>12.3</v>
@@ -2075,15 +2067,15 @@
         <v>10718715</v>
       </c>
       <c r="L42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C43">
         <v>14</v>
@@ -2092,13 +2084,13 @@
         <v>4632</v>
       </c>
       <c r="F43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I43">
         <v>6.18</v>
@@ -2110,15 +2102,15 @@
         <v>5404015</v>
       </c>
       <c r="L43" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C44">
         <v>15</v>
@@ -2127,13 +2119,13 @@
         <v>4632</v>
       </c>
       <c r="F44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I44">
         <v>0.55800000000000005</v>
@@ -2145,15 +2137,15 @@
         <v>1951875</v>
       </c>
       <c r="L44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45">
         <v>16</v>
@@ -2162,13 +2154,13 @@
         <v>4632</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I45">
         <v>0.246</v>
@@ -2180,15 +2172,15 @@
         <v>1624104</v>
       </c>
       <c r="L45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C46">
         <v>17</v>
@@ -2197,13 +2189,13 @@
         <v>4632</v>
       </c>
       <c r="F46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I46">
         <v>0.76200000000000001</v>
@@ -2215,15 +2207,15 @@
         <v>2012835</v>
       </c>
       <c r="L46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C47">
         <v>18</v>
@@ -2232,13 +2224,13 @@
         <v>4632</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I47">
         <v>5.36</v>
@@ -2250,15 +2242,15 @@
         <v>5412467</v>
       </c>
       <c r="L47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48">
         <v>19</v>
@@ -2267,13 +2259,13 @@
         <v>4632</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I48">
         <v>11.6</v>
@@ -2285,15 +2277,15 @@
         <v>10267120</v>
       </c>
       <c r="L48" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
         <v>20</v>
@@ -2302,13 +2294,13 @@
         <v>4632</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I49">
         <v>15.8</v>
@@ -2320,15 +2312,15 @@
         <v>10786416</v>
       </c>
       <c r="L49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50">
         <v>21</v>
@@ -2337,13 +2329,13 @@
         <v>4632</v>
       </c>
       <c r="F50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I50">
         <v>0.435</v>
@@ -2355,15 +2347,15 @@
         <v>1704223</v>
       </c>
       <c r="L50" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C51">
         <v>22</v>
@@ -2372,13 +2364,13 @@
         <v>4632</v>
       </c>
       <c r="F51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I51">
         <v>17.899999999999999</v>
@@ -2390,15 +2382,15 @@
         <v>8994586</v>
       </c>
       <c r="L51" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C52">
         <v>23</v>
@@ -2407,13 +2399,13 @@
         <v>4632</v>
       </c>
       <c r="F52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I52">
         <v>0.217</v>
@@ -2425,15 +2417,15 @@
         <v>761218</v>
       </c>
       <c r="L52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C53">
         <v>24</v>
@@ -2442,13 +2434,13 @@
         <v>4632</v>
       </c>
       <c r="F53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I53">
         <v>0.20599999999999999</v>
@@ -2460,7 +2452,7 @@
         <v>1652503</v>
       </c>
       <c r="L53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>